<commit_message>
commit project truoc khi push quang
</commit_message>
<xml_diff>
--- a/excel-file/nhanVien-fail-idNational-data.xlsx
+++ b/excel-file/nhanVien-fail-idNational-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse-Workspace-AdvancedTest\WolvesResApp\excel-file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kiemthu_nangcao\WolvesResApp\WolvesResApp\excel-file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA999A6-D033-4ACD-9C39-08774CA6924E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25D88D1-6AEC-4689-B659-CE0D049160C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1068" windowWidth="19452" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5328" yWindow="1908" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>

</xml_diff>